<commit_message>
Forgot to add dependencies
</commit_message>
<xml_diff>
--- a/tests/wetlab2variations_execution_nxf.variations.xlsx
+++ b/tests/wetlab2variations_execution_nxf.variations.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">params.general.rawreads</t>
   </si>
@@ -58,10 +58,25 @@
     <t xml:space="preserve">@RG\tID:HB66DADXX\tSM:NA24695\tPL:ILLUMINA</t>
   </si>
   <si>
-    <t xml:space="preserve">NA24695.g.vcf.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA24695.metrics.txt</t>
+    <t xml:space="preserve">NA24695_HB66DADXX.g.vcf.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA24695_HB66DADXX.metrics.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp://ftp-trace.ncbi.nih.gov/giab/ftp/data/ChineseTrio/HG007_NA24695-hu38168_mother/NA24695_Mother_HiSeq100x/NA24695_Mother_HiSeq100x_fastqs/141117_D00360_0066_BHB7AUADXX/Sample_NA24695/NA24695_CTTGTA_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp://ftp-trace.ncbi.nih.gov/giab/ftp/data/ChineseTrio/HG007_NA24695-hu38168_mother/NA24695_Mother_HiSeq100x/NA24695_Mother_HiSeq100x_fastqs/141117_D00360_0066_BHB7AUADXX/Sample_NA24695/NA24695_CTTGTA_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@RG\tID:HB7AUADXX\tSM:NA24695\tPL:ILLUMINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA24695_HB7AUADXX.g.vcf.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA24695_HB7AUADXX.metrics.txt</t>
   </si>
 </sst>
 </file>
@@ -76,6 +91,7 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,10 +173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.015625" defaultRowHeight="11.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -221,6 +237,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>